<commit_message>
Latest updates to metadata and processing script
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="20940" windowHeight="9600"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="20100" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="182">
   <si>
     <t>IT_50uL@5OD</t>
   </si>
@@ -440,6 +440,126 @@
   </si>
   <si>
     <t>na</t>
+  </si>
+  <si>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>M7</t>
+  </si>
+  <si>
+    <t>M8</t>
+  </si>
+  <si>
+    <t>M9</t>
+  </si>
+  <si>
+    <t>/FUS4/data2/CJM/cabiGrant/20150523</t>
+  </si>
+  <si>
+    <t>e416/s5129</t>
+  </si>
+  <si>
+    <t>e416/s5142</t>
+  </si>
+  <si>
+    <t>e416/s5156</t>
+  </si>
+  <si>
+    <t>e417/s5199</t>
+  </si>
+  <si>
+    <t>e418/s5217</t>
+  </si>
+  <si>
+    <t>e418/s5228</t>
+  </si>
+  <si>
+    <t>e418/s5239</t>
+  </si>
+  <si>
+    <t>e416/s5171</t>
+  </si>
+  <si>
+    <t>106   121    41    37</t>
+  </si>
+  <si>
+    <t>112 113 40 51</t>
+  </si>
+  <si>
+    <t>111    97    39    62</t>
+  </si>
+  <si>
+    <t>119   130    58    73</t>
+  </si>
+  <si>
+    <t>129   108    50    55</t>
+  </si>
+  <si>
+    <t>110    85    56    76</t>
+  </si>
+  <si>
+    <t>103 113 63 62</t>
+  </si>
+  <si>
+    <t>112   108    48    66</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>0 60 360 475</t>
+  </si>
+  <si>
+    <t>1 1</t>
+  </si>
+  <si>
+    <t>2 1</t>
+  </si>
+  <si>
+    <t>3 1</t>
+  </si>
+  <si>
+    <t>4 1</t>
+  </si>
+  <si>
+    <t>5 1</t>
+  </si>
+  <si>
+    <t>6 1</t>
+  </si>
+  <si>
+    <t>7 1</t>
+  </si>
+  <si>
+    <t>8 1</t>
+  </si>
+  <si>
+    <t>e416/s5121</t>
+  </si>
+  <si>
+    <t>e416/s5133</t>
+  </si>
+  <si>
+    <t>e416/s5146</t>
+  </si>
+  <si>
+    <t>e416/s5160</t>
+  </si>
+  <si>
+    <t>e417/s5184</t>
+  </si>
+  <si>
+    <t>e418/s5232</t>
+  </si>
+  <si>
+    <t>e418/s5221</t>
+  </si>
+  <si>
+    <t>e418/s5211</t>
+  </si>
+  <si>
+    <t>0 0 0 0</t>
   </si>
 </sst>
 </file>
@@ -924,8 +1044,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1268,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF8"/>
+  <dimension ref="A1:AF16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AF8" sqref="AF8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,7 +1975,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
         <v>128</v>
@@ -1916,8 +2037,14 @@
       <c r="U7" t="s">
         <v>73</v>
       </c>
+      <c r="V7" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="W7" t="s">
         <v>74</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="Y7" t="s">
         <v>88</v>
@@ -1946,7 +2073,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
         <v>129</v>
@@ -2008,9 +2135,15 @@
       <c r="U8" t="s">
         <v>86</v>
       </c>
+      <c r="V8" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="W8" t="s">
         <v>87</v>
       </c>
+      <c r="X8" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="Y8" t="s">
         <v>89</v>
       </c>
@@ -2034,6 +2167,766 @@
       </c>
       <c r="AF8" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9">
+        <v>20150523</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9">
+        <v>980</v>
+      </c>
+      <c r="F9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G9">
+        <v>1.5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>146</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="U9" t="s">
+        <v>147</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA9">
+        <v>3</v>
+      </c>
+      <c r="AB9">
+        <v>1000</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AD9">
+        <v>1</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10">
+        <v>20150523</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10">
+        <v>980</v>
+      </c>
+      <c r="F10" t="s">
+        <v>164</v>
+      </c>
+      <c r="G10">
+        <v>1.5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>146</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="U10" t="s">
+        <v>148</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA10">
+        <v>3</v>
+      </c>
+      <c r="AB10">
+        <v>1000</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AD10">
+        <v>1</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>166</v>
+      </c>
+      <c r="AF10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11">
+        <v>20150523</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11">
+        <v>980</v>
+      </c>
+      <c r="F11" t="s">
+        <v>164</v>
+      </c>
+      <c r="G11">
+        <v>1.5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>146</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="U11" t="s">
+        <v>149</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA11">
+        <v>3</v>
+      </c>
+      <c r="AB11">
+        <v>1000</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AD11">
+        <v>1</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>167</v>
+      </c>
+      <c r="AF11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12">
+        <v>20150523</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E12">
+        <v>980</v>
+      </c>
+      <c r="F12" t="s">
+        <v>164</v>
+      </c>
+      <c r="G12">
+        <v>1.5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>146</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="U12" t="s">
+        <v>154</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA12">
+        <v>3</v>
+      </c>
+      <c r="AB12">
+        <v>1000</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AD12">
+        <v>1</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>168</v>
+      </c>
+      <c r="AF12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13">
+        <v>20150523</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13">
+        <v>980</v>
+      </c>
+      <c r="F13" t="s">
+        <v>164</v>
+      </c>
+      <c r="G13">
+        <v>1.5</v>
+      </c>
+      <c r="I13" t="s">
+        <v>146</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="U13" t="s">
+        <v>150</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA13">
+        <v>3</v>
+      </c>
+      <c r="AB13">
+        <v>1000</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AD13">
+        <v>1</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>169</v>
+      </c>
+      <c r="AF13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14">
+        <v>20150523</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14">
+        <v>980</v>
+      </c>
+      <c r="F14" t="s">
+        <v>164</v>
+      </c>
+      <c r="G14">
+        <v>1.5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>146</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="U14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA14">
+        <v>3</v>
+      </c>
+      <c r="AB14">
+        <v>1000</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AD14">
+        <v>1</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15">
+        <v>20150523</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E15">
+        <v>980</v>
+      </c>
+      <c r="F15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G15">
+        <v>1.5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>146</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="U15" t="s">
+        <v>152</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA15">
+        <v>3</v>
+      </c>
+      <c r="AB15">
+        <v>1000</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AD15">
+        <v>1</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>171</v>
+      </c>
+      <c r="AF15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16">
+        <v>20150523</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16">
+        <v>980</v>
+      </c>
+      <c r="F16" t="s">
+        <v>164</v>
+      </c>
+      <c r="G16">
+        <v>1.5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>146</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="U16" t="s">
+        <v>153</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA16">
+        <v>3</v>
+      </c>
+      <c r="AB16">
+        <v>1000</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AD16">
+        <v>1</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF16">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>